<commit_message>
add more border styles, border color
</commit_message>
<xml_diff>
--- a/tests/fixtures/example.xlsx
+++ b/tests/fixtures/example.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Размеры страховых премий по договорам страхования в рамках международной системы страхования 
 «Зеленая карта», применяемые с 15 августа 2016 года по 14 сентября 2016 года</t>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>1pt</t>
+  </si>
+  <si>
+    <t>1.5pt</t>
   </si>
 </sst>
 </file>
@@ -162,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="19">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -275,6 +281,41 @@
       <bottom style="thick">
         <color rgb="FF008000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dotted"/>
+      <right style="dotted"/>
+      <top style="dotted"/>
+      <bottom style="dotted"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dashed"/>
+      <right style="dashed"/>
+      <top style="dashed"/>
+      <bottom style="dashed"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dashDotDot"/>
+      <right style="dashDotDot"/>
+      <top style="dashDotDot"/>
+      <bottom style="dashDotDot"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="double"/>
+      <right style="double"/>
+      <top style="double"/>
+      <bottom style="double"/>
       <diagonal/>
     </border>
   </borders>
@@ -303,7 +344,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -381,6 +422,26 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -401,10 +462,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:O37"/>
+  <dimension ref="B1:O47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="O:O B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1361,6 +1422,32 @@
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
       <c r="E37" s="19"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="20"/>
+      <c r="D39" s="21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D40" s="21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="22"/>
+      <c r="D41" s="21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="22"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="23"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1396,7 +1483,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O:O A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1422,7 +1509,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O:O A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
currency and color format
</commit_message>
<xml_diff>
--- a/tests/fixtures/example.xlsx
+++ b/tests/fixtures/example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="433" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="391" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Лист 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -75,9 +75,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_р_._-;\-* #,##0_р_._-;_-* \-_р_._-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ [$р.-419];\-#,##0.00\ [$р.-419]"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_р_._-;\-* #,##0_р_._-;_-* \-_р_._-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="#,###.00"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00\ [$р.-419];\-#,##0.00\ [$р.-419]"/>
+    <numFmt numFmtId="169" formatCode="[RED]0.00"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -344,7 +348,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -377,6 +381,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -413,6 +425,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -422,6 +438,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -464,8 +484,8 @@
   </sheetPr>
   <dimension ref="B1:O47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -610,91 +630,91 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="7" t="n">
         <v>2700</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="8" t="n">
         <v>5160</v>
       </c>
-      <c r="E8" s="7" t="n">
+      <c r="E8" s="8" t="n">
         <v>9590</v>
       </c>
-      <c r="F8" s="7" t="n">
+      <c r="F8" s="8" t="n">
         <v>13520</v>
       </c>
-      <c r="G8" s="7" t="n">
+      <c r="G8" s="8" t="n">
         <v>16710</v>
       </c>
-      <c r="H8" s="7" t="n">
+      <c r="H8" s="8" t="n">
         <v>18190</v>
       </c>
-      <c r="I8" s="7" t="n">
+      <c r="I8" s="8" t="n">
         <v>19660</v>
       </c>
-      <c r="J8" s="7" t="n">
+      <c r="J8" s="8" t="n">
         <v>20650</v>
       </c>
-      <c r="K8" s="7" t="n">
+      <c r="K8" s="8" t="n">
         <v>21630</v>
       </c>
-      <c r="L8" s="7" t="n">
+      <c r="L8" s="8" t="n">
         <v>22610</v>
       </c>
-      <c r="M8" s="7" t="n">
+      <c r="M8" s="8" t="n">
         <v>23350</v>
       </c>
-      <c r="N8" s="7" t="n">
+      <c r="N8" s="8" t="n">
         <v>23840</v>
       </c>
-      <c r="O8" s="7" t="n">
+      <c r="O8" s="8" t="n">
         <v>24580</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="9" t="n">
         <v>810</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D9" s="8" t="n">
         <v>1540</v>
       </c>
-      <c r="E9" s="7" t="n">
+      <c r="E9" s="8" t="n">
         <v>2870</v>
       </c>
-      <c r="F9" s="7" t="n">
+      <c r="F9" s="8" t="n">
         <v>4040</v>
       </c>
-      <c r="G9" s="7" t="n">
+      <c r="G9" s="8" t="n">
         <v>5000</v>
       </c>
-      <c r="H9" s="7" t="n">
+      <c r="H9" s="8" t="n">
         <v>5440</v>
       </c>
-      <c r="I9" s="7" t="n">
+      <c r="I9" s="8" t="n">
         <v>5880</v>
       </c>
-      <c r="J9" s="7" t="n">
+      <c r="J9" s="8" t="n">
         <v>6170</v>
       </c>
-      <c r="K9" s="7" t="n">
+      <c r="K9" s="8" t="n">
         <v>6470</v>
       </c>
-      <c r="L9" s="7" t="n">
+      <c r="L9" s="8" t="n">
         <v>6760</v>
       </c>
-      <c r="M9" s="7" t="n">
+      <c r="M9" s="8" t="n">
         <v>6980</v>
       </c>
-      <c r="N9" s="7" t="n">
+      <c r="N9" s="8" t="n">
         <v>7130</v>
       </c>
-      <c r="O9" s="7" t="n">
+      <c r="O9" s="8" t="n">
         <v>7350</v>
       </c>
     </row>
@@ -702,43 +722,43 @@
       <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="8" t="n">
         <v>4510</v>
       </c>
-      <c r="D10" s="7" t="n">
+      <c r="D10" s="8" t="n">
         <v>8610</v>
       </c>
-      <c r="E10" s="7" t="n">
+      <c r="E10" s="8" t="n">
         <v>16000</v>
       </c>
-      <c r="F10" s="7" t="n">
+      <c r="F10" s="8" t="n">
         <v>22560</v>
       </c>
-      <c r="G10" s="7" t="n">
+      <c r="G10" s="8" t="n">
         <v>27900</v>
       </c>
-      <c r="H10" s="7" t="n">
+      <c r="H10" s="8" t="n">
         <v>30360</v>
       </c>
-      <c r="I10" s="7" t="n">
+      <c r="I10" s="8" t="n">
         <v>32820</v>
       </c>
-      <c r="J10" s="7" t="n">
+      <c r="J10" s="8" t="n">
         <v>34460</v>
       </c>
-      <c r="K10" s="7" t="n">
+      <c r="K10" s="8" t="n">
         <v>36100</v>
       </c>
-      <c r="L10" s="7" t="n">
+      <c r="L10" s="8" t="n">
         <v>37740</v>
       </c>
-      <c r="M10" s="7" t="n">
+      <c r="M10" s="8" t="n">
         <v>38970</v>
       </c>
-      <c r="N10" s="7" t="n">
+      <c r="N10" s="8" t="n">
         <v>39790</v>
       </c>
-      <c r="O10" s="7" t="n">
+      <c r="O10" s="8" t="n">
         <v>41020</v>
       </c>
     </row>
@@ -746,43 +766,43 @@
       <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="8" t="n">
         <v>900</v>
       </c>
-      <c r="D11" s="7" t="n">
+      <c r="D11" s="8" t="n">
         <v>1730</v>
       </c>
-      <c r="E11" s="7" t="n">
+      <c r="E11" s="8" t="n">
         <v>3210</v>
       </c>
-      <c r="F11" s="7" t="n">
+      <c r="F11" s="8" t="n">
         <v>4520</v>
       </c>
-      <c r="G11" s="7" t="n">
+      <c r="G11" s="8" t="n">
         <v>5590</v>
       </c>
-      <c r="H11" s="7" t="n">
+      <c r="H11" s="8" t="n">
         <v>6080</v>
       </c>
-      <c r="I11" s="7" t="n">
+      <c r="I11" s="8" t="n">
         <v>6580</v>
       </c>
-      <c r="J11" s="7" t="n">
+      <c r="J11" s="8" t="n">
         <v>6910</v>
       </c>
-      <c r="K11" s="7" t="n">
+      <c r="K11" s="8" t="n">
         <v>7230</v>
       </c>
-      <c r="L11" s="7" t="n">
+      <c r="L11" s="8" t="n">
         <v>7560</v>
       </c>
-      <c r="M11" s="7" t="n">
+      <c r="M11" s="8" t="n">
         <v>7810</v>
       </c>
-      <c r="N11" s="7" t="n">
+      <c r="N11" s="8" t="n">
         <v>7970</v>
       </c>
-      <c r="O11" s="7" t="n">
+      <c r="O11" s="8" t="n">
         <v>8220</v>
       </c>
     </row>
@@ -790,43 +810,43 @@
       <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C12" s="8" t="n">
         <v>7740</v>
       </c>
-      <c r="D12" s="7" t="n">
+      <c r="D12" s="8" t="n">
         <v>13890</v>
       </c>
-      <c r="E12" s="7" t="n">
+      <c r="E12" s="8" t="n">
         <v>23040</v>
       </c>
-      <c r="F12" s="7" t="n">
+      <c r="F12" s="8" t="n">
         <v>32200</v>
       </c>
-      <c r="G12" s="7" t="n">
+      <c r="G12" s="8" t="n">
         <v>41350</v>
       </c>
-      <c r="H12" s="7" t="n">
+      <c r="H12" s="8" t="n">
         <v>50510</v>
       </c>
-      <c r="I12" s="7" t="n">
+      <c r="I12" s="8" t="n">
         <v>59660</v>
       </c>
-      <c r="J12" s="7" t="n">
+      <c r="J12" s="8" t="n">
         <v>68820</v>
       </c>
-      <c r="K12" s="7" t="n">
+      <c r="K12" s="8" t="n">
         <v>77980</v>
       </c>
-      <c r="L12" s="7" t="n">
+      <c r="L12" s="8" t="n">
         <v>87130</v>
       </c>
-      <c r="M12" s="7" t="n">
+      <c r="M12" s="8" t="n">
         <v>96290</v>
       </c>
-      <c r="N12" s="7" t="n">
+      <c r="N12" s="8" t="n">
         <v>105440</v>
       </c>
-      <c r="O12" s="7" t="n">
+      <c r="O12" s="8" t="n">
         <v>114600</v>
       </c>
     </row>
@@ -834,43 +854,43 @@
       <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="8" t="n">
         <v>1350</v>
       </c>
-      <c r="D13" s="7" t="n">
+      <c r="D13" s="8" t="n">
         <v>2580</v>
       </c>
-      <c r="E13" s="7" t="n">
+      <c r="E13" s="8" t="n">
         <v>4800</v>
       </c>
-      <c r="F13" s="7" t="n">
+      <c r="F13" s="8" t="n">
         <v>6760</v>
       </c>
-      <c r="G13" s="7" t="n">
+      <c r="G13" s="8" t="n">
         <v>8360</v>
       </c>
-      <c r="H13" s="7" t="n">
+      <c r="H13" s="8" t="n">
         <v>9100</v>
       </c>
-      <c r="I13" s="7" t="n">
+      <c r="I13" s="8" t="n">
         <v>9840</v>
       </c>
-      <c r="J13" s="7" t="n">
+      <c r="J13" s="8" t="n">
         <v>10330</v>
       </c>
-      <c r="K13" s="7" t="n">
+      <c r="K13" s="8" t="n">
         <v>10820</v>
       </c>
-      <c r="L13" s="7" t="n">
+      <c r="L13" s="8" t="n">
         <v>11310</v>
       </c>
-      <c r="M13" s="7" t="n">
+      <c r="M13" s="8" t="n">
         <v>11680</v>
       </c>
-      <c r="N13" s="7" t="n">
+      <c r="N13" s="8" t="n">
         <v>11930</v>
       </c>
-      <c r="O13" s="7" t="n">
+      <c r="O13" s="8" t="n">
         <v>12300</v>
       </c>
     </row>
@@ -878,61 +898,61 @@
       <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="7" t="n">
+      <c r="C14" s="8" t="n">
         <v>1650</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="8" t="n">
         <v>3150</v>
       </c>
-      <c r="E14" s="7" t="n">
+      <c r="E14" s="8" t="n">
         <v>5850</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="8" t="n">
         <v>8250</v>
       </c>
-      <c r="G14" s="7" t="n">
+      <c r="G14" s="8" t="n">
         <v>10200</v>
       </c>
-      <c r="H14" s="7" t="n">
+      <c r="H14" s="8" t="n">
         <v>11100</v>
       </c>
-      <c r="I14" s="7" t="n">
+      <c r="I14" s="8" t="n">
         <v>12000</v>
       </c>
-      <c r="J14" s="7" t="n">
+      <c r="J14" s="8" t="n">
         <v>12600</v>
       </c>
-      <c r="K14" s="7" t="n">
+      <c r="K14" s="8" t="n">
         <v>13200</v>
       </c>
-      <c r="L14" s="7" t="n">
+      <c r="L14" s="8" t="n">
         <v>13800</v>
       </c>
-      <c r="M14" s="7" t="n">
+      <c r="M14" s="8" t="n">
         <v>14250</v>
       </c>
-      <c r="N14" s="7" t="n">
+      <c r="N14" s="8" t="n">
         <v>14550</v>
       </c>
-      <c r="O14" s="7" t="n">
+      <c r="O14" s="8" t="n">
         <v>15000</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
@@ -1071,43 +1091,43 @@
       <c r="B24" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="7" t="n">
+      <c r="C24" s="8" t="n">
         <v>920</v>
       </c>
-      <c r="D24" s="7" t="n">
+      <c r="D24" s="8" t="n">
         <v>1230</v>
       </c>
-      <c r="E24" s="7" t="n">
+      <c r="E24" s="8" t="n">
         <v>1850</v>
       </c>
-      <c r="F24" s="7" t="n">
+      <c r="F24" s="8" t="n">
         <v>2460</v>
       </c>
-      <c r="G24" s="7" t="n">
+      <c r="G24" s="8" t="n">
         <v>3080</v>
       </c>
-      <c r="H24" s="7" t="n">
+      <c r="H24" s="8" t="n">
         <v>3690</v>
       </c>
-      <c r="I24" s="7" t="n">
+      <c r="I24" s="8" t="n">
         <v>4310</v>
       </c>
-      <c r="J24" s="7" t="n">
+      <c r="J24" s="8" t="n">
         <v>4610</v>
       </c>
-      <c r="K24" s="7" t="n">
+      <c r="K24" s="8" t="n">
         <v>4920</v>
       </c>
-      <c r="L24" s="7" t="n">
+      <c r="L24" s="8" t="n">
         <v>5230</v>
       </c>
-      <c r="M24" s="7" t="n">
+      <c r="M24" s="8" t="n">
         <v>5540</v>
       </c>
-      <c r="N24" s="7" t="n">
+      <c r="N24" s="8" t="n">
         <v>5850</v>
       </c>
-      <c r="O24" s="7" t="n">
+      <c r="O24" s="8" t="n">
         <v>6150</v>
       </c>
     </row>
@@ -1115,43 +1135,43 @@
       <c r="B25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="7" t="n">
+      <c r="C25" s="8" t="n">
         <v>280</v>
       </c>
-      <c r="D25" s="7" t="n">
+      <c r="D25" s="8" t="n">
         <v>370</v>
       </c>
-      <c r="E25" s="7" t="n">
+      <c r="E25" s="8" t="n">
         <v>550</v>
       </c>
-      <c r="F25" s="7" t="n">
+      <c r="F25" s="8" t="n">
         <v>740</v>
       </c>
-      <c r="G25" s="7" t="n">
+      <c r="G25" s="8" t="n">
         <v>920</v>
       </c>
-      <c r="H25" s="7" t="n">
+      <c r="H25" s="8" t="n">
         <v>1100</v>
       </c>
-      <c r="I25" s="7" t="n">
+      <c r="I25" s="8" t="n">
         <v>1290</v>
       </c>
-      <c r="J25" s="7" t="n">
+      <c r="J25" s="8" t="n">
         <v>1380</v>
       </c>
-      <c r="K25" s="7" t="n">
+      <c r="K25" s="8" t="n">
         <v>1470</v>
       </c>
-      <c r="L25" s="7" t="n">
+      <c r="L25" s="8" t="n">
         <v>1560</v>
       </c>
-      <c r="M25" s="7" t="n">
+      <c r="M25" s="8" t="n">
         <v>1650</v>
       </c>
-      <c r="N25" s="7" t="n">
+      <c r="N25" s="8" t="n">
         <v>1750</v>
       </c>
-      <c r="O25" s="7" t="n">
+      <c r="O25" s="8" t="n">
         <v>1840</v>
       </c>
     </row>
@@ -1159,43 +1179,43 @@
       <c r="B26" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="7" t="n">
+      <c r="C26" s="8" t="n">
         <v>1570</v>
       </c>
-      <c r="D26" s="7" t="n">
+      <c r="D26" s="8" t="n">
         <v>2090</v>
       </c>
-      <c r="E26" s="7" t="n">
+      <c r="E26" s="8" t="n">
         <v>3140</v>
       </c>
-      <c r="F26" s="7" t="n">
+      <c r="F26" s="8" t="n">
         <v>4180</v>
       </c>
-      <c r="G26" s="7" t="n">
+      <c r="G26" s="8" t="n">
         <v>5230</v>
       </c>
-      <c r="H26" s="7" t="n">
+      <c r="H26" s="8" t="n">
         <v>6270</v>
       </c>
-      <c r="I26" s="7" t="n">
+      <c r="I26" s="8" t="n">
         <v>7320</v>
       </c>
-      <c r="J26" s="7" t="n">
+      <c r="J26" s="8" t="n">
         <v>7840</v>
       </c>
-      <c r="K26" s="7" t="n">
+      <c r="K26" s="8" t="n">
         <v>8370</v>
       </c>
-      <c r="L26" s="7" t="n">
+      <c r="L26" s="8" t="n">
         <v>8890</v>
       </c>
-      <c r="M26" s="7" t="n">
+      <c r="M26" s="8" t="n">
         <v>9410</v>
       </c>
-      <c r="N26" s="7" t="n">
+      <c r="N26" s="8" t="n">
         <v>9940</v>
       </c>
-      <c r="O26" s="7" t="n">
+      <c r="O26" s="8" t="n">
         <v>10460</v>
       </c>
     </row>
@@ -1203,43 +1223,43 @@
       <c r="B27" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="7" t="n">
+      <c r="C27" s="8" t="n">
         <v>310</v>
       </c>
-      <c r="D27" s="7" t="n">
+      <c r="D27" s="8" t="n">
         <v>420</v>
       </c>
-      <c r="E27" s="7" t="n">
+      <c r="E27" s="8" t="n">
         <v>630</v>
       </c>
-      <c r="F27" s="7" t="n">
+      <c r="F27" s="8" t="n">
         <v>840</v>
       </c>
-      <c r="G27" s="7" t="n">
+      <c r="G27" s="8" t="n">
         <v>1040</v>
       </c>
-      <c r="H27" s="7" t="n">
+      <c r="H27" s="8" t="n">
         <v>1250</v>
       </c>
-      <c r="I27" s="7" t="n">
+      <c r="I27" s="8" t="n">
         <v>1460</v>
       </c>
-      <c r="J27" s="7" t="n">
+      <c r="J27" s="8" t="n">
         <v>1570</v>
       </c>
-      <c r="K27" s="7" t="n">
+      <c r="K27" s="8" t="n">
         <v>1670</v>
       </c>
-      <c r="L27" s="7" t="n">
+      <c r="L27" s="8" t="n">
         <v>1780</v>
       </c>
-      <c r="M27" s="7" t="n">
+      <c r="M27" s="8" t="n">
         <v>1880</v>
       </c>
-      <c r="N27" s="7" t="n">
+      <c r="N27" s="8" t="n">
         <v>1990</v>
       </c>
-      <c r="O27" s="7" t="n">
+      <c r="O27" s="8" t="n">
         <v>2090</v>
       </c>
     </row>
@@ -1247,43 +1267,43 @@
       <c r="B28" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="7" t="n">
+      <c r="C28" s="8" t="n">
         <v>1920</v>
       </c>
-      <c r="D28" s="7" t="n">
+      <c r="D28" s="8" t="n">
         <v>3450</v>
       </c>
-      <c r="E28" s="7" t="n">
+      <c r="E28" s="8" t="n">
         <v>5730</v>
       </c>
-      <c r="F28" s="7" t="n">
+      <c r="F28" s="8" t="n">
         <v>8010</v>
       </c>
-      <c r="G28" s="7" t="n">
+      <c r="G28" s="8" t="n">
         <v>10280</v>
       </c>
-      <c r="H28" s="7" t="n">
+      <c r="H28" s="8" t="n">
         <v>12560</v>
       </c>
-      <c r="I28" s="7" t="n">
+      <c r="I28" s="8" t="n">
         <v>14840</v>
       </c>
-      <c r="J28" s="7" t="n">
+      <c r="J28" s="8" t="n">
         <v>17110</v>
       </c>
-      <c r="K28" s="7" t="n">
+      <c r="K28" s="8" t="n">
         <v>19390</v>
       </c>
-      <c r="L28" s="7" t="n">
+      <c r="L28" s="8" t="n">
         <v>21670</v>
       </c>
-      <c r="M28" s="7" t="n">
+      <c r="M28" s="8" t="n">
         <v>23940</v>
       </c>
-      <c r="N28" s="7" t="n">
+      <c r="N28" s="8" t="n">
         <v>26220</v>
       </c>
-      <c r="O28" s="7" t="n">
+      <c r="O28" s="8" t="n">
         <v>28500</v>
       </c>
     </row>
@@ -1291,43 +1311,43 @@
       <c r="B29" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="7" t="n">
+      <c r="C29" s="8" t="n">
         <v>460</v>
       </c>
-      <c r="D29" s="7" t="n">
+      <c r="D29" s="8" t="n">
         <v>610</v>
       </c>
-      <c r="E29" s="7" t="n">
+      <c r="E29" s="8" t="n">
         <v>910</v>
       </c>
-      <c r="F29" s="7" t="n">
+      <c r="F29" s="8" t="n">
         <v>1210</v>
       </c>
-      <c r="G29" s="7" t="n">
+      <c r="G29" s="8" t="n">
         <v>1520</v>
       </c>
-      <c r="H29" s="7" t="n">
+      <c r="H29" s="8" t="n">
         <v>1820</v>
       </c>
-      <c r="I29" s="7" t="n">
+      <c r="I29" s="8" t="n">
         <v>2120</v>
       </c>
-      <c r="J29" s="7" t="n">
+      <c r="J29" s="8" t="n">
         <v>2280</v>
       </c>
-      <c r="K29" s="7" t="n">
+      <c r="K29" s="8" t="n">
         <v>2430</v>
       </c>
-      <c r="L29" s="7" t="n">
+      <c r="L29" s="8" t="n">
         <v>2580</v>
       </c>
-      <c r="M29" s="7" t="n">
+      <c r="M29" s="8" t="n">
         <v>2730</v>
       </c>
-      <c r="N29" s="7" t="n">
+      <c r="N29" s="8" t="n">
         <v>2880</v>
       </c>
-      <c r="O29" s="7" t="n">
+      <c r="O29" s="8" t="n">
         <v>3030</v>
       </c>
     </row>
@@ -1335,119 +1355,126 @@
       <c r="B30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="7" t="n">
+      <c r="C30" s="8" t="n">
         <v>560</v>
       </c>
-      <c r="D30" s="7" t="n">
+      <c r="D30" s="8" t="n">
         <v>750</v>
       </c>
-      <c r="E30" s="7" t="n">
+      <c r="E30" s="8" t="n">
         <v>1130</v>
       </c>
-      <c r="F30" s="7" t="n">
+      <c r="F30" s="8" t="n">
         <v>1500</v>
       </c>
-      <c r="G30" s="7" t="n">
+      <c r="G30" s="8" t="n">
         <v>1880</v>
       </c>
-      <c r="H30" s="7" t="n">
+      <c r="H30" s="8" t="n">
         <v>2260</v>
       </c>
-      <c r="I30" s="7" t="n">
+      <c r="I30" s="8" t="n">
         <v>2630</v>
       </c>
-      <c r="J30" s="7" t="n">
+      <c r="J30" s="8" t="n">
         <v>2820</v>
       </c>
-      <c r="K30" s="7" t="n">
+      <c r="K30" s="8" t="n">
         <v>3010</v>
       </c>
-      <c r="L30" s="7" t="n">
+      <c r="L30" s="8" t="n">
         <v>3200</v>
       </c>
-      <c r="M30" s="7" t="n">
+      <c r="M30" s="8" t="n">
         <v>3380</v>
       </c>
-      <c r="N30" s="7" t="n">
+      <c r="N30" s="8" t="n">
         <v>3570</v>
       </c>
-      <c r="O30" s="7" t="n">
+      <c r="O30" s="8" t="n">
         <v>3760</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="10"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="14"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="14"/>
+      <c r="E33" s="16"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="16"/>
-      <c r="E35" s="14"/>
+      <c r="B35" s="18"/>
+      <c r="E35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="16"/>
-      <c r="E36" s="14"/>
+      <c r="B36" s="19" t="n">
+        <v>24545</v>
+      </c>
+      <c r="E36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="17"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="19"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="22"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="23" t="n">
+        <v>1234</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="20"/>
-      <c r="D39" s="21" t="s">
+      <c r="B39" s="24"/>
+      <c r="D39" s="25" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="21" t="s">
+      <c r="D40" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="22"/>
-      <c r="D41" s="21" t="s">
+      <c r="B41" s="26"/>
+      <c r="D41" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="22"/>
+      <c r="B43" s="26"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="23"/>
+      <c r="B45" s="27"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="24"/>
+      <c r="B47" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>

<commit_message>
fix for indexed color
</commit_message>
<xml_diff>
--- a/tests/fixtures/example.xlsx
+++ b/tests/fixtures/example.xlsx
@@ -348,7 +348,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -419,10 +419,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -474,6 +470,11 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -484,8 +485,8 @@
   </sheetPr>
   <dimension ref="B1:O47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1430,51 +1431,54 @@
       <c r="E34" s="17"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="18"/>
+      <c r="B35" s="18" t="n">
+        <f aca="false">B36+D30</f>
+        <v>25295</v>
+      </c>
       <c r="E35" s="16"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="19" t="n">
+      <c r="B36" s="18" t="n">
         <v>24545</v>
       </c>
       <c r="E36" s="16"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="20"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="22"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="21"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E38" s="23" t="n">
+      <c r="E38" s="22" t="n">
         <v>1234</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="24"/>
-      <c r="D39" s="25" t="s">
+      <c r="B39" s="23"/>
+      <c r="D39" s="24" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="25" t="s">
+      <c r="D40" s="24" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="26"/>
-      <c r="D41" s="25" t="s">
+      <c r="B41" s="25"/>
+      <c r="D41" s="24" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="26"/>
+      <c r="B43" s="25"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="27"/>
+      <c r="B45" s="26"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="28"/>
+      <c r="B47" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1492,6 +1496,11 @@
     <mergeCell ref="B31:O31"/>
     <mergeCell ref="B34:E34"/>
   </mergeCells>
+  <conditionalFormatting sqref="C24:I30">
+    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>1000</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Simple work with images
</commit_message>
<xml_diff>
--- a/tests/fixtures/example.xlsx
+++ b/tests/fixtures/example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="391" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Лист 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,62 +13,64 @@
     <sheet name="Лист3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
-  <si>
-    <t>Размеры страховых премий по договорам страхования в рамках международной системы страхования 
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+  <si>
+    <t xml:space="preserve">Размеры страховых премий по договорам страхования в рамках международной системы страхования 
 «Зеленая карта», применяемые с 15 августа 2016 года по 14 сентября 2016 года</t>
   </si>
   <si>
-    <t>Размеры страховых премий по международному страхованию гражданской ответственности владельцев транспортных средств «Зеленая карта» для территории действия «Все страны системы «Зеленая карта» (рублей).</t>
-  </si>
-  <si>
-    <t>Применяются с «15» августа 2016 года до «14» сентября 2016 года включительно</t>
-  </si>
-  <si>
-    <t>Тип транспортного средства</t>
-  </si>
-  <si>
-    <t>Срок страхования, месяцев</t>
-  </si>
-  <si>
-    <t>15 дней</t>
-  </si>
-  <si>
-    <t>Легковые автомобили</t>
-  </si>
-  <si>
-    <t>Прицепы к легковым автомобилям</t>
-  </si>
-  <si>
-    <t>Грузовые автомобили, тягачи</t>
-  </si>
-  <si>
-    <t>Прицепы и полуприцепы к грузовым автомобилям и тягачам</t>
-  </si>
-  <si>
-    <t>Автобусы</t>
-  </si>
-  <si>
-    <t>Мотоциклы, мотороллеры, мотоколяски и мопеды</t>
-  </si>
-  <si>
-    <t>Сельскохозяйственная и строительная техника</t>
-  </si>
-  <si>
-    <t>Размеры страховых тарифов по международному страхованию гражданской ответственности владельцев транспортных средств «Зеленая карта» для территории действия «Республика Беларусь, Республика Молдова, Украина и Азербайджанская Республика» (рублей).</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>1pt</t>
-  </si>
-  <si>
-    <t>1.5pt</t>
+    <t xml:space="preserve">Размеры страховых премий по международному страхованию гражданской ответственности владельцев транспортных средств «Зеленая карта» для территории действия «Все страны системы «Зеленая карта» (рублей).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Применяются с «15» августа 2016 года до «14» сентября 2016 года включительно</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Тип транспортного средства</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Срок страхования, месяцев</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 дней</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Легковые автомобили</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Прицепы к легковым автомобилям</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Грузовые автомобили, тягачи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Прицепы и полуприцепы к грузовым автомобилям и тягачам</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Автобусы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мотоциклы, мотороллеры, мотоколяски и мопеды</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сельскохозяйственная и строительная техника</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5pt</t>
   </si>
 </sst>
 </file>
@@ -76,7 +78,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="10">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$р.-419];\-#,##0.00\ [$р.-419]"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0_р_._-;\-* #,##0_р_._-;_-* \-_р_._-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="#,###.00"/>
@@ -87,7 +89,7 @@
     <numFmt numFmtId="172" formatCode="HH:MM:SS\ AM/PM"/>
     <numFmt numFmtId="173" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -149,13 +151,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF800000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -352,7 +347,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -397,10 +392,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -413,7 +404,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -483,18 +474,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -503,20 +489,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:O47"/>
+  <dimension ref="B1:O1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.71255060728745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.85425101214575"/>
-    <col collapsed="false" hidden="false" max="14" min="4" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.40485829959514"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.5748987854251"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="4" style="0" width="8.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="8.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -975,574 +961,122 @@
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
     </row>
-    <row r="16" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="38.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="55.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="2" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-    </row>
-    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-    </row>
-    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="4"/>
-      <c r="C23" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F23" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="G23" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="H23" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="I23" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="J23" s="5" t="n">
-        <v>7</v>
-      </c>
-      <c r="K23" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="L23" s="5" t="n">
-        <v>9</v>
-      </c>
-      <c r="M23" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="N23" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="O23" s="5" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="8" t="n">
-        <v>920</v>
-      </c>
-      <c r="D24" s="8" t="n">
-        <v>1230</v>
-      </c>
-      <c r="E24" s="8" t="n">
-        <v>1850</v>
-      </c>
-      <c r="F24" s="8" t="n">
-        <v>2460</v>
-      </c>
-      <c r="G24" s="8" t="n">
-        <v>3080</v>
-      </c>
-      <c r="H24" s="8" t="n">
-        <v>3690</v>
-      </c>
-      <c r="I24" s="8" t="n">
-        <v>4310</v>
-      </c>
-      <c r="J24" s="8" t="n">
-        <v>4610</v>
-      </c>
-      <c r="K24" s="8" t="n">
-        <v>4920</v>
-      </c>
-      <c r="L24" s="8" t="n">
-        <v>5230</v>
-      </c>
-      <c r="M24" s="8" t="n">
-        <v>5540</v>
-      </c>
-      <c r="N24" s="8" t="n">
-        <v>5850</v>
-      </c>
-      <c r="O24" s="8" t="n">
-        <v>6150</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="8" t="n">
-        <v>280</v>
-      </c>
-      <c r="D25" s="8" t="n">
-        <v>370</v>
-      </c>
-      <c r="E25" s="8" t="n">
-        <v>550</v>
-      </c>
-      <c r="F25" s="8" t="n">
-        <v>740</v>
-      </c>
-      <c r="G25" s="8" t="n">
-        <v>920</v>
-      </c>
-      <c r="H25" s="8" t="n">
-        <v>1100</v>
-      </c>
-      <c r="I25" s="8" t="n">
-        <v>1290</v>
-      </c>
-      <c r="J25" s="8" t="n">
-        <v>1380</v>
-      </c>
-      <c r="K25" s="8" t="n">
-        <v>1470</v>
-      </c>
-      <c r="L25" s="8" t="n">
-        <v>1560</v>
-      </c>
-      <c r="M25" s="8" t="n">
-        <v>1650</v>
-      </c>
-      <c r="N25" s="8" t="n">
-        <v>1750</v>
-      </c>
-      <c r="O25" s="8" t="n">
-        <v>1840</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="8" t="n">
-        <v>1570</v>
-      </c>
-      <c r="D26" s="8" t="n">
-        <v>2090</v>
-      </c>
-      <c r="E26" s="8" t="n">
-        <v>3140</v>
-      </c>
-      <c r="F26" s="8" t="n">
-        <v>4180</v>
-      </c>
-      <c r="G26" s="8" t="n">
-        <v>5230</v>
-      </c>
-      <c r="H26" s="8" t="n">
-        <v>6270</v>
-      </c>
-      <c r="I26" s="8" t="n">
-        <v>7320</v>
-      </c>
-      <c r="J26" s="8" t="n">
-        <v>7840</v>
-      </c>
-      <c r="K26" s="8" t="n">
-        <v>8370</v>
-      </c>
-      <c r="L26" s="8" t="n">
-        <v>8890</v>
-      </c>
-      <c r="M26" s="8" t="n">
-        <v>9410</v>
-      </c>
-      <c r="N26" s="8" t="n">
-        <v>9940</v>
-      </c>
-      <c r="O26" s="8" t="n">
-        <v>10460</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="8" t="n">
-        <v>310</v>
-      </c>
-      <c r="D27" s="8" t="n">
-        <v>420</v>
-      </c>
-      <c r="E27" s="8" t="n">
-        <v>630</v>
-      </c>
-      <c r="F27" s="8" t="n">
-        <v>840</v>
-      </c>
-      <c r="G27" s="8" t="n">
-        <v>1040</v>
-      </c>
-      <c r="H27" s="8" t="n">
-        <v>1250</v>
-      </c>
-      <c r="I27" s="8" t="n">
-        <v>1460</v>
-      </c>
-      <c r="J27" s="8" t="n">
-        <v>1570</v>
-      </c>
-      <c r="K27" s="8" t="n">
-        <v>1670</v>
-      </c>
-      <c r="L27" s="8" t="n">
-        <v>1780</v>
-      </c>
-      <c r="M27" s="8" t="n">
-        <v>1880</v>
-      </c>
-      <c r="N27" s="8" t="n">
-        <v>1990</v>
-      </c>
-      <c r="O27" s="8" t="n">
-        <v>2090</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="8" t="n">
-        <v>1920</v>
-      </c>
-      <c r="D28" s="8" t="n">
-        <v>3450</v>
-      </c>
-      <c r="E28" s="8" t="n">
-        <v>5730</v>
-      </c>
-      <c r="F28" s="8" t="n">
-        <v>8010</v>
-      </c>
-      <c r="G28" s="8" t="n">
-        <v>10280</v>
-      </c>
-      <c r="H28" s="8" t="n">
-        <v>12560</v>
-      </c>
-      <c r="I28" s="8" t="n">
-        <v>14840</v>
-      </c>
-      <c r="J28" s="8" t="n">
-        <v>17110</v>
-      </c>
-      <c r="K28" s="8" t="n">
-        <v>19390</v>
-      </c>
-      <c r="L28" s="8" t="n">
-        <v>21670</v>
-      </c>
-      <c r="M28" s="8" t="n">
-        <v>23940</v>
-      </c>
-      <c r="N28" s="8" t="n">
-        <v>26220</v>
-      </c>
-      <c r="O28" s="8" t="n">
-        <v>28500</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="8" t="n">
-        <v>460</v>
-      </c>
-      <c r="D29" s="8" t="n">
-        <v>610</v>
-      </c>
-      <c r="E29" s="8" t="n">
-        <v>910</v>
-      </c>
-      <c r="F29" s="8" t="n">
-        <v>1210</v>
-      </c>
-      <c r="G29" s="8" t="n">
-        <v>1520</v>
-      </c>
-      <c r="H29" s="8" t="n">
-        <v>1820</v>
-      </c>
-      <c r="I29" s="8" t="n">
-        <v>2120</v>
-      </c>
-      <c r="J29" s="8" t="n">
-        <v>2280</v>
-      </c>
-      <c r="K29" s="8" t="n">
-        <v>2430</v>
-      </c>
-      <c r="L29" s="8" t="n">
-        <v>2580</v>
-      </c>
-      <c r="M29" s="8" t="n">
-        <v>2730</v>
-      </c>
-      <c r="N29" s="8" t="n">
-        <v>2880</v>
-      </c>
-      <c r="O29" s="8" t="n">
-        <v>3030</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="8" t="n">
-        <v>560</v>
-      </c>
-      <c r="D30" s="8" t="n">
-        <v>750</v>
-      </c>
-      <c r="E30" s="8" t="n">
-        <v>1130</v>
-      </c>
-      <c r="F30" s="8" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G30" s="8" t="n">
-        <v>1880</v>
-      </c>
-      <c r="H30" s="8" t="n">
-        <v>2260</v>
-      </c>
-      <c r="I30" s="8" t="n">
-        <v>2630</v>
-      </c>
-      <c r="J30" s="8" t="n">
-        <v>2820</v>
-      </c>
-      <c r="K30" s="8" t="n">
-        <v>3010</v>
-      </c>
-      <c r="L30" s="8" t="n">
-        <v>3200</v>
-      </c>
-      <c r="M30" s="8" t="n">
-        <v>3380</v>
-      </c>
-      <c r="N30" s="8" t="n">
-        <v>3570</v>
-      </c>
-      <c r="O30" s="8" t="n">
-        <v>3760</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="12"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="14"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="15" t="s">
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="17" t="e">
+        <f aca="false">B20+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="17" t="n">
+        <v>24545</v>
+      </c>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="21" t="n">
+        <f aca="true">NOW()</f>
+        <v>44077.6559523308</v>
+      </c>
+      <c r="E22" s="22" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="23" t="n">
+        <f aca="true">NOW()</f>
+        <v>44077.655952331</v>
+      </c>
+      <c r="D23" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="16"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="18" t="n">
-        <f aca="false">B36+D30</f>
-        <v>25295</v>
-      </c>
-      <c r="E35" s="16"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="18" t="n">
-        <v>24545</v>
-      </c>
-      <c r="E36" s="16"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="21"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="22" t="n">
-        <f aca="true">NOW()</f>
-        <v>42620.9135004709</v>
-      </c>
-      <c r="E38" s="23" t="n">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="24" t="n">
-        <f aca="true">NOW()</f>
-        <v>42620.9135004712</v>
-      </c>
-      <c r="D39" s="25" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="25" t="n">
+        <f aca="true">TODAY()</f>
+        <v>44077</v>
+      </c>
+      <c r="D24" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="26" t="n">
-        <f aca="true">TODAY()</f>
-        <v>42620</v>
-      </c>
-      <c r="D40" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="27" t="n">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="26" t="n">
         <v>0.9046875</v>
       </c>
-      <c r="D41" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="28" t="n">
-        <f aca="false">B41- TIME(1, 0, 0)</f>
+      <c r="D25" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="27" t="n">
+        <f aca="false">B25- TIME(1, 0, 0)</f>
         <v>0.863020833333333</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="29"/>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="30"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="31"/>
-    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="28"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="29"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="30"/>
+    </row>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="7">
     <mergeCell ref="B1:O2"/>
     <mergeCell ref="B3:O3"/>
     <mergeCell ref="B5:O5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:O6"/>
     <mergeCell ref="B15:O15"/>
-    <mergeCell ref="B16:O17"/>
-    <mergeCell ref="B19:O19"/>
-    <mergeCell ref="B21:O21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:O22"/>
-    <mergeCell ref="B31:O31"/>
-    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B18:E18"/>
   </mergeCells>
-  <conditionalFormatting sqref="C24:I30">
-    <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>1000</formula>
-    </cfRule>
-  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1557,18 +1091,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.58"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1583,18 +1117,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.58"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
process implement diagonal border; update tests; reformat
</commit_message>
<xml_diff>
--- a/tests/fixtures/example.xlsx
+++ b/tests/fixtures/example.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t xml:space="preserve">Размеры страховых премий по договорам страхования в рамках международной системы страхования 
 «Зеленая карта», применяемые с 15 августа 2016 года по 14 сентября 2016 года</t>
@@ -71,6 +71,153 @@
   </si>
   <si>
     <t xml:space="preserve">1.5pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V and H align</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Border</t>
+  </si>
+  <si>
+    <t xml:space="preserve">left-top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center-top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right-top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.05pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">left-center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center-center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right-center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dotted</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1s 1l d</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left-bottom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center-bottom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right-bottom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L dash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s dash</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2 pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">double</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2s 1l d</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3 pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left indent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagonal border</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text rotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90 degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">270 degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45 degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">315 degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">180 degrees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Border collapse issue with merged cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text decoration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">underline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">italic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ubi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">u double</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shadow effect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outline effect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shadow and outline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text wrap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">long text foo bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wrap long text</t>
   </si>
 </sst>
 </file>
@@ -89,7 +236,7 @@
     <numFmt numFmtId="172" formatCode="HH:MM:SS\ AM/PM"/>
     <numFmt numFmtId="173" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -156,8 +303,83 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <strike val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <u val="double"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <shadow val="true"/>
+      <sz val="16"/>
+      <color rgb="FFFF9966"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <outline val="true"/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <outline val="true"/>
+      <shadow val="true"/>
+      <sz val="15"/>
+      <color rgb="FFFF8080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,11 +389,29 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFE6E64C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6E64C"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CC66"/>
+        <bgColor rgb="FF00AE00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="27">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -320,6 +560,68 @@
       <top style="double"/>
       <bottom style="double"/>
       <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="dashDot"/>
+      <right style="dashDot"/>
+      <top style="dashDot"/>
+      <bottom style="dashDot"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thick"/>
+      <right style="thick"/>
+      <top style="thick"/>
+      <bottom style="thick"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="true" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="thin"/>
+    </border>
+    <border diagonalUp="true" diagonalDown="true">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="thin"/>
+    </border>
+    <border diagonalUp="false" diagonalDown="true">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="thin"/>
+    </border>
+    <border diagonalUp="true" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal style="thin">
+        <color rgb="FF00AE00"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="true" diagonalDown="true">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal style="thin">
+        <color rgb="FF00AE00"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="false" diagonalDown="true">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal style="thin">
+        <color rgb="FF00AE00"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="20">
@@ -347,7 +649,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="76">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -470,6 +772,186 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="5" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="135" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -481,6 +963,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFE6E64C"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF9966"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CC66"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF00AE00"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -491,8 +1033,8 @@
   </sheetPr>
   <dimension ref="B1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -500,9 +1042,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="4" style="0" width="8.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="4" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="8.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1001,7 +1543,7 @@
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="21" t="n">
         <f aca="true">NOW()</f>
-        <v>44077.6559523308</v>
+        <v>44360.4641731851</v>
       </c>
       <c r="E22" s="22" t="n">
         <v>1234</v>
@@ -1010,7 +1552,7 @@
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="23" t="n">
         <f aca="true">NOW()</f>
-        <v>44077.655952331</v>
+        <v>44360.4641731856</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>14</v>
@@ -1019,7 +1561,7 @@
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="25" t="n">
         <f aca="true">TODAY()</f>
-        <v>44077</v>
+        <v>44360</v>
       </c>
       <c r="D24" s="24" t="s">
         <v>15</v>
@@ -1089,17 +1631,444 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="B1:N44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.6"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="I2" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="33"/>
+      <c r="D3" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="34"/>
+      <c r="F3" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="35"/>
+      <c r="I3" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="37"/>
+      <c r="D5" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="38"/>
+      <c r="F5" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="39"/>
+      <c r="I5" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="42"/>
+      <c r="D7" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="43"/>
+      <c r="F7" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="44"/>
+      <c r="I7" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I9" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" s="48" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="I11" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="I13" s="52"/>
+      <c r="K13" s="53"/>
+      <c r="M13" s="54"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I14" s="52"/>
+      <c r="K14" s="53"/>
+      <c r="M14" s="54"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="38"/>
+      <c r="I16" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="K16" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="M16" s="61" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="38"/>
+      <c r="I17" s="59"/>
+      <c r="K17" s="60"/>
+      <c r="M17" s="61"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="38"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="38"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="55"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="38"/>
+      <c r="I20" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" s="62"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="62"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I21" s="62"/>
+      <c r="J21" s="62"/>
+      <c r="K21" s="62"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="62"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="64"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="66" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="67" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="J23" s="64"/>
+      <c r="K23" s="63"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="J25" s="64"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="72" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="J26" s="64"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="74" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="74"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="74"/>
+      <c r="C29" s="74"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="24.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="75" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="37">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="F3:G4"/>
+    <mergeCell ref="B5:C6"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="F5:G6"/>
+    <mergeCell ref="B7:C8"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="F7:G8"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="I11:M11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="D16:D20"/>
+    <mergeCell ref="E16:E20"/>
+    <mergeCell ref="F16:G20"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="I20:M20"/>
+    <mergeCell ref="I21:M21"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="J22:J26"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="B26:D27"/>
+    <mergeCell ref="E26:G27"/>
+    <mergeCell ref="B28:G29"/>
+    <mergeCell ref="B32:G32"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1117,13 +2086,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.6"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>